<commit_message>
migrations and view updates
</commit_message>
<xml_diff>
--- a/alexander_matheson/final_project/Schema Design.xlsx
+++ b/alexander_matheson/final_project/Schema Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="600" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="16580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="135">
   <si>
     <t>locations_start</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>*********</t>
-  </si>
-  <si>
-    <t>photo</t>
   </si>
   <si>
     <t>.png</t>
@@ -958,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1016,7 +1013,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>2</v>
@@ -1046,7 +1043,7 @@
         <v>77</v>
       </c>
       <c r="X3" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Z3" s="11" t="s">
         <v>2</v>
@@ -1058,16 +1055,16 @@
         <v>76</v>
       </c>
       <c r="AC3" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD3" s="12" t="s">
         <v>74</v>
       </c>
       <c r="AE3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF3" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="AF3" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="AG3" s="12" t="s">
         <v>71</v>
@@ -1099,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -1127,13 +1124,13 @@
         <v>63</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z4" s="1">
         <v>1</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AB4" s="2" t="b">
         <v>1</v>
@@ -1175,10 +1172,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M5" s="1">
         <v>2</v>
@@ -1206,13 +1203,13 @@
         <v>64</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z5" s="1">
         <v>2</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB5" s="2" t="b">
         <v>1</v>
@@ -1242,10 +1239,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M6" s="1">
         <v>3</v>
@@ -1273,13 +1270,13 @@
         <v>65</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z6" s="1">
         <v>3</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB6" s="2" t="b">
         <v>0</v>
@@ -1305,10 +1302,10 @@
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M7" s="1">
         <v>4</v>
@@ -1336,7 +1333,7 @@
         <v>66</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z7" s="1">
         <v>4</v>
@@ -1364,10 +1361,10 @@
         <v>5</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M8" s="1">
         <v>5</v>
@@ -1391,7 +1388,7 @@
         <v>67</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z8" s="1">
         <v>5</v>
@@ -1412,10 +1409,10 @@
         <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M9" s="1">
         <v>6</v>
@@ -1439,7 +1436,7 @@
         <v>16</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z9" s="1">
         <v>6</v>
@@ -1463,7 +1460,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M10" s="1">
         <v>7</v>
@@ -1482,7 +1479,7 @@
         <v>68</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z10" s="1">
         <v>7</v>
@@ -1506,7 +1503,7 @@
         <v>46</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M11" s="1">
         <v>8</v>
@@ -1525,7 +1522,7 @@
         <v>69</v>
       </c>
       <c r="X11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z11" s="1">
         <v>8</v>
@@ -1549,7 +1546,7 @@
         <v>60</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M12" s="1">
         <v>9</v>
@@ -1566,7 +1563,7 @@
       </c>
       <c r="W12" s="2"/>
       <c r="X12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z12" s="4">
         <v>9</v>
@@ -1598,7 +1595,7 @@
       </c>
       <c r="W13" s="2"/>
       <c r="X13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:36">
@@ -1627,7 +1624,7 @@
       </c>
       <c r="W14" s="2"/>
       <c r="X14" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:36">
@@ -1653,10 +1650,10 @@
         <v>80</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M15" s="1">
         <v>12</v>
@@ -1673,7 +1670,7 @@
       </c>
       <c r="W15" s="2"/>
       <c r="X15" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:36">
@@ -1699,10 +1696,10 @@
         <v>26</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M16" s="1">
         <v>15</v>
@@ -1719,11 +1716,11 @@
       </c>
       <c r="W16" s="2"/>
       <c r="X16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z16" s="15"/>
       <c r="AA16" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AB16" s="16"/>
       <c r="AC16" s="16"/>
@@ -1769,22 +1766,22 @@
       </c>
       <c r="W17" s="2"/>
       <c r="X17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z17" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA17" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="AA17" s="2" t="s">
+      <c r="AB17" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AB17" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="AC17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AD17" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="AD17" s="3" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:30">
@@ -1827,16 +1824,16 @@
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z18" s="1">
         <v>1</v>
       </c>
       <c r="AA18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB18" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="AB18" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" s="3"/>
@@ -1881,7 +1878,7 @@
       </c>
       <c r="W19" s="2"/>
       <c r="X19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z19" s="1">
         <v>2</v>
@@ -1931,7 +1928,7 @@
       </c>
       <c r="W20" s="2"/>
       <c r="X20" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z20" s="1">
         <v>3</v>
@@ -1967,7 +1964,7 @@
       </c>
       <c r="W21" s="5"/>
       <c r="X21" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Z21" s="4">
         <v>4</v>
@@ -2061,10 +2058,10 @@
     </row>
     <row r="28" spans="1:30">
       <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" t="s">
         <v>107</v>
-      </c>
-      <c r="D28" t="s">
-        <v>108</v>
       </c>
       <c r="M28" s="1">
         <v>27</v>
@@ -2079,10 +2076,10 @@
     </row>
     <row r="29" spans="1:30">
       <c r="B29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M29" s="1">
         <v>28</v>
@@ -2100,7 +2097,7 @@
         <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M30" s="1">
         <v>29</v>
@@ -2115,10 +2112,10 @@
     </row>
     <row r="31" spans="1:30">
       <c r="B31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M31" s="1">
         <v>30</v>
@@ -2136,7 +2133,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M32" s="1">
         <v>31</v>
@@ -2151,10 +2148,10 @@
     </row>
     <row r="33" spans="2:16">
       <c r="B33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M33" s="1">
         <v>32</v>
@@ -2169,10 +2166,10 @@
     </row>
     <row r="34" spans="2:16">
       <c r="B34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M34" s="1">
         <v>33</v>
@@ -2187,10 +2184,10 @@
     </row>
     <row r="35" spans="2:16">
       <c r="B35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M35" s="1">
         <v>34</v>
@@ -2205,7 +2202,7 @@
     </row>
     <row r="36" spans="2:16">
       <c r="D36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M36" s="1">
         <v>35</v>
@@ -2220,7 +2217,7 @@
     </row>
     <row r="37" spans="2:16">
       <c r="D37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M37" s="1">
         <v>36</v>
@@ -2235,7 +2232,7 @@
     </row>
     <row r="38" spans="2:16">
       <c r="D38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M38" s="1">
         <v>37</v>
@@ -2250,7 +2247,7 @@
     </row>
     <row r="39" spans="2:16">
       <c r="D39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M39" s="1">
         <v>38</v>
@@ -2265,7 +2262,7 @@
     </row>
     <row r="40" spans="2:16">
       <c r="D40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M40" s="1">
         <v>39</v>

</xml_diff>